<commit_message>
More data for India
</commit_message>
<xml_diff>
--- a/FoundData/IndiaDataInvestigation.xlsx
+++ b/FoundData/IndiaDataInvestigation.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ian/Documents/GBAD/Data Quality Insights Project Folder/GBADsDataQualityInsights/FoundData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F600CD04-AAD5-7047-A0AF-4C41493BC109}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{843039B3-3D6E-8346-9109-DDC693E175A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{06B6E3E6-BCAE-D84B-A43C-2929DC10FE97}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="105">
   <si>
     <t>Country</t>
   </si>
@@ -162,13 +162,202 @@
   </si>
   <si>
     <t>FAOSTAT is reporting identical cattle population for this year as Vikaspedia (Ministry of Electronics and Information Technology) is for this year. Most likely because FAOSTAT is reporting Vikaspedia's data or they both have the same source.</t>
+  </si>
+  <si>
+    <t>In 1993, India had a severe storm which caused flooding to a large portion of the country. Millions of people lost their houses and large swaths of farmland were flooded. We might expect to see an impact on the cattle population during this time. However, the country is so massive and there is so many cattle in India that even though the flooding was severe, it did not flood enough of the country to have a meaningful impact on the population. There was a drop in the cattle population but it was part of a longer term trend.</t>
+  </si>
+  <si>
+    <t>https://reliefweb.int/report/india/india-floods-16-jul-1993-un-dha-information-reports-1-5</t>
+  </si>
+  <si>
+    <t>Chickens, Pigs, Sheep</t>
+  </si>
+  <si>
+    <t>In 1993, India had a severe storm which caused flooding to a large portion of the country. Millions of people lost their houses and large swaths of farmland were flooded. We might expect to see an impact on the sheep, chicken, and pig population during this time. However, the country is so massive and there is so much livestock that even though there was severe flooding, much of the country remained flood free. So for all the livestock that were killed, there was so much safe livestock that was able to make up for the loss.</t>
+  </si>
+  <si>
+    <t>https://reliefweb.int/report/india/india-floods-16-jul-1993-un-dha-information-reports-1-6</t>
+  </si>
+  <si>
+    <t>Cattle, Pigs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In 1973, India faced a very severe drought and as a result a famine. Just two years prior India had become food self sufficient but was now forced to import grain from the United States to feed its citizens. Some areas had to undergo restrictions for howmuch water the citizens could drink. Given all these factors, we would expect to see a drop in the livestock given the lack of water, and lack of food from not enough rain. For cattle and pigs which require lots of water and food, we see a reduction in the population for this year. This is good evidence for FAOSTATs data quality given the climate conditions at the time. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">In 1973, India faced a very severe drought and as a result a famine. Just two years prior India had become food self sufficient but was now forced to import grain from the United States to feed its citizens. Some areas had to undergo restrictions for howmuch water the citizens could drink. Given all these factors, we would expect to see a drop in the livestock given the lack of water, and lack of food from not enough rain. For chickens the population increases for this year. This would appear to be bad data however, deeper investigation into where most chicken farming occurs in India, a majority of the chickens grown in the country do not occur in the most affected areas. So given this FAOSTATs data is plausible.  </t>
+  </si>
+  <si>
+    <t>https://www.nytimes.com/1973/02/20/archives/worst-drought-in-decade-perils-indias-food-supply-worst-drought-in.html</t>
+  </si>
+  <si>
+    <t>https://www.nytimes.com/1973/02/20/archives/worst-drought-in-decade-perils-indias-food-supply-worst-drought-in.html, https://www.statista.com/statistics/622738/poultry-inventory-by-state-india/</t>
+  </si>
+  <si>
+    <t>https://www.nytimes.com/1973/02/20/archives/worst-drought-in-decade-perils-indias-food-supply-worst-drought-in.html, https://www.statista.com/statistics/622738/poultry-inventory-by-state-india/, https://dahd.nic.in/sites/default/filess/NAP%20on%20Sheep.pdf</t>
+  </si>
+  <si>
+    <t>In 1973, India faced a very severe drought and as a result a famine. Just two years prior India had become food self sufficient but was now forced to import grain from the United States to feed its citizens. Some areas had to undergo restrictions for howmuch water the citizens could drink. Given all these factors, we would expect to see a drop in the livestock given the lack of water, and lack of food from not enough rain. For sheep the population increases for this year. This would appear to be bad data however, deeper investigation into where most sheep farming occurs in India, a majority of the sheep grown in the country occur in the north-western and southern peninsula of the country which were less affected by the drought. Sheep are also more hardy towards drought being able to consume more fiberous foods which would allow them to handle the drought better.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2002, 2009, 2012, </t>
+  </si>
+  <si>
+    <t>In 2002, 2009, and 2012, India had weather conditions that caused drought. Since India has a history of droughts occuring, the Indian government has done more to prep the country so droughts are less impactful to people. They have saved up food and built better water management systems. As a result we would expect to see less of an impact on the livestock as reported by FAOSTAT. FAOSTAT shows almost no impact during these drought years on any livestock which makes sense given the Indian governments prepardness.</t>
+  </si>
+  <si>
+    <t>1996-1997</t>
+  </si>
+  <si>
+    <t>https://www.downtoearth.org.in/news/food/india-claims-to-be-self-sufficient-in-food-production-but-facts-say-otherwise-62091</t>
+  </si>
+  <si>
+    <t>In 1996, The Andhra Pradesh cyclone struck India. This powerful cyclone killed around 1000 people and flooded many areas of the Andhra Pradesh state. It only lasted two days inland but caused deaths to many livestock in it's path. Given the severity of the cyclone and its path in the middle of the country where farming is more common we would expect to see it impact the livestock populations of the country. The chicken population during this time was on an almost constant increase. However, in 1997, the year after the cyclone took place, the population dropped. Given that the cyclone occured in November, this is good evidence that it impacted the population and is why FAOSTAT recorded a smaller population in 1996</t>
+  </si>
+  <si>
+    <t>In 1996, The Andhra Pradesh cyclone struck India. This powerful cyclone killed around 1000 people and flooded many areas of the Andhra Pradesh state. It only lasted two days inland but caused deaths to many livestock in it's path. Given the severity of the cyclone and its path in the middle of the country where farming is more common we would expect to see it impact the livestock populations of the country. The cattle population for this year shows a decline which makes sense given the severe storm and flooding. However, the decline of these years was part of a larger trend of a shrinking cattle population so it can be hard to determine how much of this decline was caused by the storm.</t>
+  </si>
+  <si>
+    <t>https://www.google.com/url?sa=t&amp;rct=j&amp;q=&amp;esrc=s&amp;source=web&amp;cd=&amp;ved=2ahUKEwjjhPqhhfyEAxXt_skDHerXCQMQFnoECBEQAQ&amp;url=https%3A%2F%2Fmausamjournal.imd.gov.in%2Findex.php%2FMAUSAM%2Farticle%2Fdownload%2F1816%2F1629%2F6886&amp;usg=AOvVaw29fEKVec72qB29wPhwCKVB&amp;opi=89978449</t>
+  </si>
+  <si>
+    <t>Sheep, Pigs</t>
+  </si>
+  <si>
+    <t>In 1996, The Andhra Pradesh cyclone struck India. This powerful cyclone killed around 1000 people and flooded many areas of the Andhra Pradesh state. It only lasted two days inland but caused deaths to many livestock in it's path. Given the severity of the cyclone and its path in the middle of the country where farming is more common we would expect to see it impact the livestock populations of the country. FAOSTAT reports increasing populations for sheep and pigs for these. This is plausible because the states that grow the most pigs and sheep were not located in the path of the cyclone.</t>
+  </si>
+  <si>
+    <t>https://www.google.com/url?sa=t&amp;rct=j&amp;q=&amp;esrc=s&amp;source=web&amp;cd=&amp;ved=2ahUKEwjjhPqhhfyEAxXt_skDHerXCQMQFnoECBEQAQ&amp;url=https%3A%2F%2Fmausamjournal.imd.gov.in%2Findex.php%2FMAUSAM%2Farticle%2Fdownload%2F1816%2F1629%2F6886&amp;usg=AOvVaw29fEKVec72qB29wPhwCKVB&amp;opi=89978449, https://www.google.com/url?sa=t&amp;rct=j&amp;q=&amp;esrc=s&amp;source=web&amp;cd=&amp;cad=rja&amp;uact=8&amp;ved=2ahUKEwijhNLoivyEAxXtLdAFHVvTABsQFnoECHIQAQ&amp;url=https%3A%2F%2Fdahd.nic.in%2Fsites%2Fdefault%2Ffiless%2FNAP%2520on%2520Sheep.pdf&amp;usg=AOvVaw1sWrMyy1EVopE7x7by88Z0&amp;opi=89978449, https://www.google.com/url?sa=t&amp;rct=j&amp;q=&amp;esrc=s&amp;source=web&amp;cd=&amp;ved=2ahUKEwjYs5TGivyEAxWU5skDHV0ABM8QFnoECA4QAw&amp;url=https%3A%2F%2Fwww.pig333.com%2Flatest_swine_news%2Fpork-production-in-india_11587%2F%23%3A~%3Atext%3DThe%2520eastern%2520and%2520north%2520eastern%2CWest%2520Bengal%2520(0.65%2520million).&amp;usg=AOvVaw0D4V2fsJc-OmjLyJlkORvR&amp;opi=89978449</t>
+  </si>
+  <si>
+    <t>In 2007 Cyclone Sidr made landfall in India and Bangladesh killing up to 10,000 people depending on estimates. The areas impacted in India farm a large percentage of the countries pork. As a result we would expect to see an impact on the pork population numbers. FAOSTAT shows a general decreasing population trend over this time. However, for 2007, the drop was larger than the drop in population in 2008. This makes sense given the storm that occured in the area this year.</t>
+  </si>
+  <si>
+    <t>https://reliefweb.int/report/bangladesh/cyclone-sidr-bangladesh-damage-loss-and-needs-assessment-disaster-recovery-and</t>
+  </si>
+  <si>
+    <t>In 2019 Cyclone Fani made contact with India in the state of Odisha. It caused 8.1 billion dollars USD in damages. The state has relatily small amounts of livestock with around 5 percent of the countries livestock. Given this, we wouldn't expect there to be a huge impact on the FAOSTAT numbers because the state has such a low percent of the countries livestock. FAOSTAT shows almost no impact on the populations.</t>
+  </si>
+  <si>
+    <t>https://reliefweb.int/disaster/tc-2019-000041-ind, https://odishaahvs.nic.in/upload/files/Livestock%20Biodiversity%20of%20Odisha.pdf</t>
+  </si>
+  <si>
+    <t>1980-1985</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In 1980, India implemented the Integrated Rural Development Program which was created to support the rural population so they could grow more food and livestock to increase their income and production. This was done by supplying identified groups with financial aid and supporting secondary and tertiary sectors that the farmers would rely on. Given this support we would expect the livestock population to increase in the following 5 years as farmers were able to increase their livestock population sizes with the new support from their government. For all four studied species saw their populations increase in the five years after this policy was implemented. This increase was part of an already existing trend of increasing livestock populations however so it can be hard to determine impact of this policy is on the FAOSTAT population numbers. </t>
+  </si>
+  <si>
+    <t>https://odishaahvs.nic.in/upload/files/Livestock%20Biodiversity%20of%20Odisha.pdf</t>
+  </si>
+  <si>
+    <t>1970-2000</t>
+  </si>
+  <si>
+    <t>In 1970 India launched operation Flood with the goal of increasing milk production heavily so consumers could get affordable milk. It was a large success resulting in India becoming the largest producer of dairy in the world and doubling its production by 2000. Given this we would expect to see a large increase in the cattle population between 1970 and 2000. FAOSTAT shows an increase of around 30 million cows or 15 % increase in just over 20 years. The population starts to drop after 1991. This could seem suspitious given there was a large increase for the last 20 years but makes sense given Indias growing industrialization and adoption of tractors. This allowed them to move away from using cows to pull plows and carts. Indian farmers also started renting cows instead of owning them to plow small farm fields because it became to costly to own a cow or pair of cows for the small amount of labour they did. Given this information the FAOSTAT data appears to be accurate.</t>
+  </si>
+  <si>
+    <t>https://artsandculture.google.com/story/india’s-white-revolution/DAWxXC89x_fUEA?hl=en, https://www.jstor.org/stable/24481788</t>
+  </si>
+  <si>
+    <t>1985-2003</t>
+  </si>
+  <si>
+    <t>As part of operation flood, in 1985 India start performing more artifical insemination (AI) on its cattle to product high quality cattle and milk producers. This allows the cattle to be high producers so farmers require less cows to produce the same amount of milk. Given this, we would expect to see the population of cattle decline as less of them were required to produce the same amount of outputs. FAOSTAT shows a increase in the half decade after the AI introduction but then the cattle population decreases which is a result of cattle becoming more productive.</t>
+  </si>
+  <si>
+    <t>http://naas.org.in/Policy%20Papers/policy%2096.pdf</t>
+  </si>
+  <si>
+    <t>2013-2020</t>
+  </si>
+  <si>
+    <t>Cattle, Sheep</t>
+  </si>
+  <si>
+    <t>In 2013, the Indian parlement approved the National Livestock plan whos goal was to bolster the livestock sector of the Indian economy. They outlied key areas that were hurting farmers and helped them overcome them in a sustainable way. Issues such as improving the availability of food for livestock, increasing animal productivity, improving livestock health, improving infrastructure related to getting them to market and more. Given this big effort to improve the livestock sector we would expect to see the populations increase for livestock after 2013. FAOSTAT reports the population dropping in 2014, then increasing afterwards for multiple years. This makes sense because sometimes for goals as large as this, it can take time to get suppor to farmers and start seeing results sothe 2014 drop makes sense and then the subsiquent rise afterwards is explained by the new policy.</t>
+  </si>
+  <si>
+    <t>https://dahd.nic.in/sites/default/filess/NLP%202013%20Final11.pdf</t>
+  </si>
+  <si>
+    <t>In 2013, the Indian parlement approved the National Livestock plan whos goal was to bolster the livestock sector of the Indian economy. They outlied key areas that were hurting farmers and helped them overcome them in a sustainable way. Issues such as improving the availability of food for livestock, increasing animal productivity, improving livestock health, improving infrastructure related to getting them to market and more. Given this big effort to improve the livestock sector we would expect to see the populations increase for livestock after 2013. FAOSTAT reports the population increasing every year post and including 2013. This makes sense given the new policy. However, the chicken population had already been increasing for some time so it cannot be easily determined what effect this had on the population growth.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In 2013, the Indian parlement approved the National Livestock plan whos goal was to bolster the livestock sector of the Indian economy. They outlied key areas that were hurting farmers and helped them overcome them in a sustainable way. Issues such as improving the availability of food for livestock, increasing animal productivity, improving livestock health, improving infrastructure related to getting them to market and more. Given this big effort to improve the livestock sector we would expect to see the populations increase for livestock after 2013. FAOSTAT reports the population decreasing every year after 2003 and not improving even after this bill was passed. There is no improvement to the population size even though the other studied livestock all show positive increases in the populations. </t>
+  </si>
+  <si>
+    <t>2014-2020</t>
+  </si>
+  <si>
+    <t>In 2014, India implemented the National Livestock Mission.  It's goal was to increase implement in small animal farming, and increase the productivity of the animals. Given this push, we would expect to see an increase in the animal populations (Sheep, Chickens, and Pigs) as that was the targeted animal groups for this mission. Sheep saw an increase in population starting in 2015 that continued through 2019 which aligns with this mission.</t>
+  </si>
+  <si>
+    <t>In 2014, India implemented the National Livestock Mission.  It's goal was to increase implement in small animal farming, and increase the productivity of the animals. Given this push, we would expect to see an increase in the animal populations (Sheep, Chickens, and Pigs) as that was the targeted animal groups for this mission. Chickens saw an increase every year since and this was implemented. The chicken population had already been increasing however so it cannot be easily determined the effect this had on FAOSTATs data.</t>
+  </si>
+  <si>
+    <t>In 2014, India implemented the National Livestock Mission.  It's goal was to increase implement in small animal farming, and increase the productivity of the animals. Given this push, we would expect to see an increase in the animal populations (Sheep, Chickens, and Pigs) as that was the targeted animal groups for this mission. Pigs saw a decline in their population over this time. This is suprising because the other two animal groups outlined in this mission saw an increase in their populations after this was introduced.</t>
+  </si>
+  <si>
+    <t>https://pib.gov.in/Pressreleaseshare.aspx?PRID=1781374</t>
+  </si>
+  <si>
+    <t>2014+</t>
+  </si>
+  <si>
+    <t>2010+</t>
+  </si>
+  <si>
+    <t>In 2014 India launched the National Program for Bovine Breeding and Dairy development. This program had the goal of breeding better cattle for dairy development. It is hard to know if the population should increase or decrease given this information. If the cattle are more productive, there wouldn't be a need to have as many dairy cows so we would expect the population to decrease. If instead the cows became cheaper to own or improved their life expectancy, we would expect to see more as people could have more of them. So it cannot be determined what impact this would have on the population</t>
+  </si>
+  <si>
+    <t>2005+</t>
+  </si>
+  <si>
+    <t>https://dahd.nic.in/sites/default/filess/NPBB%20Details%20and%20Scheme.pdf</t>
+  </si>
+  <si>
+    <t>https://dahd.nic.in/related-links/livestock-insurance#:~:text=Livestock%20Insurance%20Scheme%3A&amp;text=Under%20the%20scheme%2C%20the%20crossbred,to%20the%20tune%20of%2050%25.</t>
+  </si>
+  <si>
+    <t>https://vikaspedia.in/agriculture/policies-and-schemes/livestock-poultry-related/dairy-entrepreneurship-development-scheme#:~:text=During%20June%202010%2C%20the%20Dairy,2010.</t>
+  </si>
+  <si>
+    <t>In 2005 India launched the Livestock Insurance Scheme wich insured cattle and buffaloes incase they died. This provided support to farmers. Given this, we would expect to see an increase in the population numbers as now if a cow died, farmers could afford another one easier which would drive up the demand and then the supply for cows. We see an increase in the cattle population following this schemes introduction but then the population starts falling. This is supprising as it would be expected to continue to rise as farmers now had more security for their livestock.</t>
+  </si>
+  <si>
+    <t>In 2010 India launched the Dairy Entrepreneurship Development Scheme which was a Venture Capital Fund to fund new farmers wanting to start dairy farms. Given this new support and funding mechaism for new dairy farmers, we would expect to see an increase in the cattle population. Although there is not a clear outline of how successful this project was, we should still see an uptick in the cattle population. However, after it's implementation, the cattle population continued to fall according to FAOSTAT.</t>
+  </si>
+  <si>
+    <t>1965-1967</t>
+  </si>
+  <si>
+    <t>1983-1984</t>
+  </si>
+  <si>
+    <t>1990-1993</t>
+  </si>
+  <si>
+    <t>https://datacommons.org/place/country/IND?utm_medium=explore&amp;mprop=amount&amp;popt=EconomicActivity&amp;cpv=activitySource,GrossDomesticProduction&amp;hl=en</t>
+  </si>
+  <si>
+    <t>During this time period India went through a recession. Typically consumers react by buying less meat and eating more grains and affordable calories or protein. However, 8/10 Indians already limit meat consumption and 4 in 10 consider themselves vegetarian. So the effect of further limitation would probably have minimal effects on the livestock. Given hypothesis, there should be minimal impact on the livestock populations during these recessions. FAOSTAT shows little or no change in the populations during this time. This would be possible given the hypothesis of Indians already limiting their diet of meat so they would not change it much given a change in their economy.</t>
+  </si>
+  <si>
+    <t>Chickens, Pigs, Cattle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In 2020 India, along with the rest of the world, went into a recession due to the COVID-19 pandemic. Recessions usually cause people to cut back on meat consumption due to reduced income, uncertainty in the market, or other costs have risen. IN the past recessions there has been little impact on the sheep population. For the 2020 recession there was large drop in sheep. This was most likely because consumers around the world were buying less clothing and sheeps are sometimes grown for their wool. So it's possible that this is the cause of the reduction in the sheep population for this year. </t>
+  </si>
+  <si>
+    <t>https://datacommons.org/place/country/IND?utm_medium=explore&amp;mprop=amount&amp;popt=EconomicActivity&amp;cpv=activitySource,GrossDomesticProduction&amp;hl=en, https://repository.lsu.edu/cgi/viewcontent.cgi?article=1000&amp;context=textile_pubs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -181,6 +370,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Abadi"/>
     </font>
   </fonts>
   <fills count="2">
@@ -200,13 +402,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -519,10 +725,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{667C67A2-212C-B54B-A255-847972F5A21F}">
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:G59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="250" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="250" workbookViewId="0">
+      <selection activeCell="F60" sqref="F60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1220,8 +1426,675 @@
         <v>27</v>
       </c>
     </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>7</v>
+      </c>
+      <c r="B31" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31">
+        <v>1993</v>
+      </c>
+      <c r="D31" t="s">
+        <v>13</v>
+      </c>
+      <c r="E31">
+        <v>5</v>
+      </c>
+      <c r="F31" t="s">
+        <v>42</v>
+      </c>
+      <c r="G31" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>7</v>
+      </c>
+      <c r="B32" t="s">
+        <v>44</v>
+      </c>
+      <c r="C32">
+        <v>1993</v>
+      </c>
+      <c r="D32" t="s">
+        <v>13</v>
+      </c>
+      <c r="E32">
+        <v>5</v>
+      </c>
+      <c r="F32" t="s">
+        <v>45</v>
+      </c>
+      <c r="G32" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>7</v>
+      </c>
+      <c r="B33" t="s">
+        <v>47</v>
+      </c>
+      <c r="C33">
+        <v>1973</v>
+      </c>
+      <c r="D33" t="s">
+        <v>13</v>
+      </c>
+      <c r="E33">
+        <v>5</v>
+      </c>
+      <c r="F33" t="s">
+        <v>48</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>7</v>
+      </c>
+      <c r="B34" t="s">
+        <v>21</v>
+      </c>
+      <c r="C34">
+        <v>1973</v>
+      </c>
+      <c r="D34" t="s">
+        <v>13</v>
+      </c>
+      <c r="E34">
+        <v>3</v>
+      </c>
+      <c r="F34" t="s">
+        <v>49</v>
+      </c>
+      <c r="G34" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>7</v>
+      </c>
+      <c r="B35" t="s">
+        <v>18</v>
+      </c>
+      <c r="C35">
+        <v>1973</v>
+      </c>
+      <c r="D35" t="s">
+        <v>13</v>
+      </c>
+      <c r="E35">
+        <v>4</v>
+      </c>
+      <c r="F35" t="s">
+        <v>53</v>
+      </c>
+      <c r="G35" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>7</v>
+      </c>
+      <c r="B36" t="s">
+        <v>9</v>
+      </c>
+      <c r="C36" t="s">
+        <v>54</v>
+      </c>
+      <c r="D36" t="s">
+        <v>13</v>
+      </c>
+      <c r="E36">
+        <v>5</v>
+      </c>
+      <c r="F36" t="s">
+        <v>55</v>
+      </c>
+      <c r="G36" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>7</v>
+      </c>
+      <c r="B37" t="s">
+        <v>21</v>
+      </c>
+      <c r="C37" t="s">
+        <v>56</v>
+      </c>
+      <c r="D37" t="s">
+        <v>13</v>
+      </c>
+      <c r="E37">
+        <v>5</v>
+      </c>
+      <c r="F37" t="s">
+        <v>58</v>
+      </c>
+      <c r="G37" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>7</v>
+      </c>
+      <c r="B38" t="s">
+        <v>8</v>
+      </c>
+      <c r="C38" t="s">
+        <v>56</v>
+      </c>
+      <c r="D38" t="s">
+        <v>13</v>
+      </c>
+      <c r="E38">
+        <v>4</v>
+      </c>
+      <c r="F38" t="s">
+        <v>59</v>
+      </c>
+      <c r="G38" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>7</v>
+      </c>
+      <c r="B39" t="s">
+        <v>61</v>
+      </c>
+      <c r="C39" t="s">
+        <v>56</v>
+      </c>
+      <c r="D39" t="s">
+        <v>13</v>
+      </c>
+      <c r="E39">
+        <v>4</v>
+      </c>
+      <c r="F39" t="s">
+        <v>62</v>
+      </c>
+      <c r="G39" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>7</v>
+      </c>
+      <c r="B40" t="s">
+        <v>20</v>
+      </c>
+      <c r="C40">
+        <v>2007</v>
+      </c>
+      <c r="D40" t="s">
+        <v>13</v>
+      </c>
+      <c r="E40">
+        <v>5</v>
+      </c>
+      <c r="F40" t="s">
+        <v>64</v>
+      </c>
+      <c r="G40" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>7</v>
+      </c>
+      <c r="B41" t="s">
+        <v>9</v>
+      </c>
+      <c r="C41">
+        <v>2019</v>
+      </c>
+      <c r="D41" t="s">
+        <v>13</v>
+      </c>
+      <c r="E41">
+        <v>5</v>
+      </c>
+      <c r="F41" t="s">
+        <v>66</v>
+      </c>
+      <c r="G41" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>7</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C42" t="s">
+        <v>68</v>
+      </c>
+      <c r="D42" t="s">
+        <v>13</v>
+      </c>
+      <c r="E42">
+        <v>5</v>
+      </c>
+      <c r="F42" t="s">
+        <v>69</v>
+      </c>
+      <c r="G42" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>7</v>
+      </c>
+      <c r="B43" t="s">
+        <v>8</v>
+      </c>
+      <c r="C43" t="s">
+        <v>71</v>
+      </c>
+      <c r="D43" t="s">
+        <v>13</v>
+      </c>
+      <c r="E43">
+        <v>5</v>
+      </c>
+      <c r="F43" t="s">
+        <v>72</v>
+      </c>
+      <c r="G43" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>7</v>
+      </c>
+      <c r="B44" t="s">
+        <v>8</v>
+      </c>
+      <c r="C44" t="s">
+        <v>74</v>
+      </c>
+      <c r="D44" t="s">
+        <v>13</v>
+      </c>
+      <c r="E44">
+        <v>5</v>
+      </c>
+      <c r="F44" t="s">
+        <v>75</v>
+      </c>
+      <c r="G44" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>7</v>
+      </c>
+      <c r="B45" t="s">
+        <v>78</v>
+      </c>
+      <c r="C45" t="s">
+        <v>77</v>
+      </c>
+      <c r="D45" t="s">
+        <v>13</v>
+      </c>
+      <c r="E45">
+        <v>5</v>
+      </c>
+      <c r="F45" t="s">
+        <v>79</v>
+      </c>
+      <c r="G45" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>7</v>
+      </c>
+      <c r="B46" t="s">
+        <v>21</v>
+      </c>
+      <c r="C46" t="s">
+        <v>77</v>
+      </c>
+      <c r="D46" t="s">
+        <v>13</v>
+      </c>
+      <c r="E46">
+        <v>5</v>
+      </c>
+      <c r="F46" t="s">
+        <v>81</v>
+      </c>
+      <c r="G46" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>7</v>
+      </c>
+      <c r="B47" t="s">
+        <v>20</v>
+      </c>
+      <c r="C47" t="s">
+        <v>77</v>
+      </c>
+      <c r="D47" t="s">
+        <v>13</v>
+      </c>
+      <c r="E47">
+        <v>1</v>
+      </c>
+      <c r="F47" t="s">
+        <v>82</v>
+      </c>
+      <c r="G47" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>7</v>
+      </c>
+      <c r="B48" t="s">
+        <v>18</v>
+      </c>
+      <c r="C48" t="s">
+        <v>83</v>
+      </c>
+      <c r="D48" t="s">
+        <v>13</v>
+      </c>
+      <c r="E48">
+        <v>5</v>
+      </c>
+      <c r="F48" t="s">
+        <v>84</v>
+      </c>
+      <c r="G48" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>7</v>
+      </c>
+      <c r="B49" t="s">
+        <v>21</v>
+      </c>
+      <c r="C49" t="s">
+        <v>83</v>
+      </c>
+      <c r="D49" t="s">
+        <v>13</v>
+      </c>
+      <c r="E49">
+        <v>5</v>
+      </c>
+      <c r="F49" t="s">
+        <v>85</v>
+      </c>
+      <c r="G49" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>7</v>
+      </c>
+      <c r="B50" t="s">
+        <v>20</v>
+      </c>
+      <c r="C50" t="s">
+        <v>83</v>
+      </c>
+      <c r="D50" t="s">
+        <v>13</v>
+      </c>
+      <c r="E50">
+        <v>1</v>
+      </c>
+      <c r="F50" t="s">
+        <v>86</v>
+      </c>
+      <c r="G50" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>7</v>
+      </c>
+      <c r="B51" t="s">
+        <v>8</v>
+      </c>
+      <c r="C51" t="s">
+        <v>88</v>
+      </c>
+      <c r="D51" t="s">
+        <v>13</v>
+      </c>
+      <c r="F51" t="s">
+        <v>90</v>
+      </c>
+      <c r="G51" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>7</v>
+      </c>
+      <c r="B52" t="s">
+        <v>8</v>
+      </c>
+      <c r="C52" t="s">
+        <v>89</v>
+      </c>
+      <c r="D52" t="s">
+        <v>13</v>
+      </c>
+      <c r="E52">
+        <v>1</v>
+      </c>
+      <c r="F52" t="s">
+        <v>96</v>
+      </c>
+      <c r="G52" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>7</v>
+      </c>
+      <c r="B53" t="s">
+        <v>8</v>
+      </c>
+      <c r="C53" t="s">
+        <v>91</v>
+      </c>
+      <c r="D53" t="s">
+        <v>13</v>
+      </c>
+      <c r="E53">
+        <v>3</v>
+      </c>
+      <c r="F53" t="s">
+        <v>95</v>
+      </c>
+      <c r="G53" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>7</v>
+      </c>
+      <c r="B54" t="s">
+        <v>9</v>
+      </c>
+      <c r="C54" t="s">
+        <v>97</v>
+      </c>
+      <c r="D54" t="s">
+        <v>13</v>
+      </c>
+      <c r="E54">
+        <v>4</v>
+      </c>
+      <c r="F54" t="s">
+        <v>101</v>
+      </c>
+      <c r="G54" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>7</v>
+      </c>
+      <c r="B55" t="s">
+        <v>9</v>
+      </c>
+      <c r="C55" t="s">
+        <v>98</v>
+      </c>
+      <c r="D55" t="s">
+        <v>13</v>
+      </c>
+      <c r="E55">
+        <v>4</v>
+      </c>
+      <c r="F55" t="s">
+        <v>101</v>
+      </c>
+      <c r="G55" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>7</v>
+      </c>
+      <c r="B56" t="s">
+        <v>9</v>
+      </c>
+      <c r="C56" t="s">
+        <v>99</v>
+      </c>
+      <c r="D56" t="s">
+        <v>13</v>
+      </c>
+      <c r="E56">
+        <v>4</v>
+      </c>
+      <c r="F56" t="s">
+        <v>101</v>
+      </c>
+      <c r="G56" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>7</v>
+      </c>
+      <c r="B57" t="s">
+        <v>9</v>
+      </c>
+      <c r="C57">
+        <v>2008</v>
+      </c>
+      <c r="D57" t="s">
+        <v>13</v>
+      </c>
+      <c r="E57">
+        <v>4</v>
+      </c>
+      <c r="F57" t="s">
+        <v>101</v>
+      </c>
+      <c r="G57" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>7</v>
+      </c>
+      <c r="B58" t="s">
+        <v>102</v>
+      </c>
+      <c r="C58">
+        <v>2020</v>
+      </c>
+      <c r="D58" t="s">
+        <v>13</v>
+      </c>
+      <c r="E58">
+        <v>4</v>
+      </c>
+      <c r="F58" t="s">
+        <v>101</v>
+      </c>
+      <c r="G58" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>7</v>
+      </c>
+      <c r="B59" t="s">
+        <v>18</v>
+      </c>
+      <c r="C59">
+        <v>2020</v>
+      </c>
+      <c r="D59" t="s">
+        <v>13</v>
+      </c>
+      <c r="E59">
+        <v>5</v>
+      </c>
+      <c r="F59" t="s">
+        <v>103</v>
+      </c>
+      <c r="G59" t="s">
+        <v>104</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="G33" r:id="rId1" xr:uid="{C48A840E-7C7D-954F-814D-9CC8086A3F85}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>